<commit_message>
Add figure with the proposed procedure
</commit_message>
<xml_diff>
--- a/metric_means_KMEANS_3clusters.xlsx
+++ b/metric_means_KMEANS_3clusters.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20175334\Documents\PycharmProjects\monte_carlo_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984D37DA-0995-40E9-9122-E53AEF44F854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E819435-7E3F-401D-80EC-FB44B3E7B2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="metric_means_KMEANS_3clusters" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="metric_means_KMEANS_3clusters" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="24">
   <si>
     <t>cluster</t>
   </si>
@@ -73,12 +75,36 @@
   <si>
     <t>y_prime</t>
   </si>
+  <si>
+    <t>Cluster 1 (Cloudy)</t>
+  </si>
+  <si>
+    <t>Cluster 2 (Overcast)</t>
+  </si>
+  <si>
+    <t>Cluster 3 (Sunny)</t>
+  </si>
+  <si>
+    <t>Norm.</t>
+  </si>
+  <si>
+    <t>Prob. metric</t>
+  </si>
+  <si>
+    <t>Meteo. metric</t>
+  </si>
+  <si>
+    <t>CSI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +235,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -602,6 +643,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -647,7 +715,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -656,23 +724,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1028,11 +1153,1250 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4342B8BF-6010-4EB9-B6B2-100D4AF52613}">
+  <dimension ref="B1:L14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+    </row>
+    <row r="2" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+    </row>
+    <row r="3" spans="2:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="35">
+        <v>0.40693877551020402</v>
+      </c>
+      <c r="E4" s="36">
+        <v>0.28826530612244899</v>
+      </c>
+      <c r="F4" s="35">
+        <v>0.63551020408163195</v>
+      </c>
+      <c r="G4" s="35">
+        <v>0.50813559322033897</v>
+      </c>
+      <c r="H4" s="36">
+        <v>0.22906779661016899</v>
+      </c>
+      <c r="I4" s="35">
+        <v>0.69805084745762702</v>
+      </c>
+      <c r="J4" s="35">
+        <v>0.62040229885057396</v>
+      </c>
+      <c r="K4" s="36">
+        <v>0.42339080459770101</v>
+      </c>
+      <c r="L4" s="35">
+        <v>0.52126436781609198</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="31"/>
+      <c r="C5" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="37">
+        <v>3.3478881648663E-2</v>
+      </c>
+      <c r="E5" s="28">
+        <v>2.1846556638083499E-2</v>
+      </c>
+      <c r="F5" s="37">
+        <v>5.43953492350637E-2</v>
+      </c>
+      <c r="G5" s="37">
+        <v>3.2396523384897298E-2</v>
+      </c>
+      <c r="H5" s="28">
+        <v>1.7171336125926601E-2</v>
+      </c>
+      <c r="I5" s="37">
+        <v>5.3247231717396003E-2</v>
+      </c>
+      <c r="J5" s="37">
+        <v>4.8131507134494399E-2</v>
+      </c>
+      <c r="K5" s="28">
+        <v>3.07782721144347E-2</v>
+      </c>
+      <c r="L5" s="37">
+        <v>3.8775704713500503E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="35">
+        <v>0.42030612244897902</v>
+      </c>
+      <c r="E6" s="36">
+        <v>0.26989795918367299</v>
+      </c>
+      <c r="F6" s="35">
+        <v>0.70214285714285696</v>
+      </c>
+      <c r="G6" s="35">
+        <v>0.33754237288135502</v>
+      </c>
+      <c r="H6" s="36">
+        <v>0.27296610169491498</v>
+      </c>
+      <c r="I6" s="35">
+        <v>0.77584745762711804</v>
+      </c>
+      <c r="J6" s="35">
+        <v>0.465574712643678</v>
+      </c>
+      <c r="K6" s="36">
+        <v>0.30235632183908001</v>
+      </c>
+      <c r="L6" s="35">
+        <v>0.57316091954022896</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="31"/>
+      <c r="C7" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="37">
+        <v>0.77799826094604196</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0.62020439783213899</v>
+      </c>
+      <c r="F7" s="37">
+        <v>1.5828214388510999</v>
+      </c>
+      <c r="G7" s="37">
+        <v>0.62251552075899197</v>
+      </c>
+      <c r="H7" s="28">
+        <v>0.44406453157364301</v>
+      </c>
+      <c r="I7" s="37">
+        <v>1.7128279287707799</v>
+      </c>
+      <c r="J7" s="37">
+        <v>0.90678588131344495</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0.58275001748431798</v>
+      </c>
+      <c r="L7" s="37">
+        <v>1.50771928421722</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.442653061224489</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.30397959183673401</v>
+      </c>
+      <c r="F8" s="23">
+        <v>0.86918367346938696</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.32313559322033802</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0.31101694915254202</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0.89593220338983004</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0.39936781609195399</v>
+      </c>
+      <c r="K8" s="24">
+        <v>0.221954022988505</v>
+      </c>
+      <c r="L8" s="23">
+        <v>0.77224137931034398</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="23">
+        <v>3.4571210016614298E-2</v>
+      </c>
+      <c r="E9" s="24">
+        <v>2.6167073600870599E-2</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0.10117314187762599</v>
+      </c>
+      <c r="G9" s="23">
+        <v>2.3734918246323799E-2</v>
+      </c>
+      <c r="H9" s="24">
+        <v>1.7048962960689501E-2</v>
+      </c>
+      <c r="I9" s="23">
+        <v>9.5535675882812796E-2</v>
+      </c>
+      <c r="J9" s="23">
+        <v>3.1698973584203698E-2</v>
+      </c>
+      <c r="K9" s="24">
+        <v>2.1398556397482501E-2</v>
+      </c>
+      <c r="L9" s="23">
+        <v>8.7171942648499395E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0.421122448979591</v>
+      </c>
+      <c r="E10" s="36">
+        <v>0.25040816326530602</v>
+      </c>
+      <c r="F10" s="35">
+        <v>0.73163265306122405</v>
+      </c>
+      <c r="G10" s="36">
+        <v>0.234237288135593</v>
+      </c>
+      <c r="H10" s="35">
+        <v>0.32618644067796598</v>
+      </c>
+      <c r="I10" s="35">
+        <v>0.81449152542372805</v>
+      </c>
+      <c r="J10" s="35">
+        <v>0.269597701149425</v>
+      </c>
+      <c r="K10" s="36">
+        <v>0.22103448275862</v>
+      </c>
+      <c r="L10" s="35">
+        <v>0.64477011494252801</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="C11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.13711927129367199</v>
+      </c>
+      <c r="E11" s="28">
+        <v>9.3415915168832395E-2</v>
+      </c>
+      <c r="F11" s="37">
+        <v>0.27602277931192498</v>
+      </c>
+      <c r="G11" s="28">
+        <v>7.1697541106708104E-2</v>
+      </c>
+      <c r="H11" s="37">
+        <v>8.83832328389757E-2</v>
+      </c>
+      <c r="I11" s="37">
+        <v>0.26632559557493901</v>
+      </c>
+      <c r="J11" s="37">
+        <v>6.6735051407192603E-2</v>
+      </c>
+      <c r="K11" s="28">
+        <v>5.6989336459083398E-2</v>
+      </c>
+      <c r="L11" s="37">
+        <v>0.17943107792865501</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0.145654580981328</v>
+      </c>
+      <c r="E12" s="27">
+        <v>6.0892314372557502E-2</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0.139381241858445</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0.102619004688063</v>
+      </c>
+      <c r="H12" s="27">
+        <v>6.4423007573025604E-2</v>
+      </c>
+      <c r="I12" s="29">
+        <v>9.2577533357374606E-2</v>
+      </c>
+      <c r="J12" s="29">
+        <v>6.2416238689166001E-2</v>
+      </c>
+      <c r="K12" s="27">
+        <v>4.39508437270726E-2</v>
+      </c>
+      <c r="L12" s="29">
+        <v>5.8095500122279202E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="41"/>
+      <c r="C13" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="33">
+        <v>5.3495188061392598E-2</v>
+      </c>
+      <c r="E13" s="34">
+        <v>3.5257503348294299E-2</v>
+      </c>
+      <c r="F13" s="33">
+        <v>5.1142718350508098E-2</v>
+      </c>
+      <c r="G13" s="33">
+        <v>4.3617524972792199E-2</v>
+      </c>
+      <c r="H13" s="34">
+        <v>2.8451457536020502E-2</v>
+      </c>
+      <c r="I13" s="33">
+        <v>4.25760552874902E-2</v>
+      </c>
+      <c r="J13" s="33">
+        <v>2.8953443445941099E-2</v>
+      </c>
+      <c r="K13" s="34">
+        <v>2.4955302053384299E-2</v>
+      </c>
+      <c r="L13" s="33">
+        <v>2.79823518034557E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C6928C-2D4C-44A9-AAA3-545755DB95FF}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="14" customWidth="1"/>
+    <col min="3" max="11" width="5.85546875" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.40693877551020402</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.28826530612244899</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.63551020408163195</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.50813559322033897</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0.22906779661016899</v>
+      </c>
+      <c r="H4" s="16">
+        <v>0.69805084745762702</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.62040229885057396</v>
+      </c>
+      <c r="J4" s="22">
+        <v>0.42339080459770101</v>
+      </c>
+      <c r="K4" s="16">
+        <v>0.52126436781609198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3.3478881648663E-2</v>
+      </c>
+      <c r="D5" s="22">
+        <v>2.1846556638083499E-2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5.43953492350637E-2</v>
+      </c>
+      <c r="F5" s="16">
+        <v>3.2396523384897298E-2</v>
+      </c>
+      <c r="G5" s="22">
+        <v>1.7171336125926601E-2</v>
+      </c>
+      <c r="H5" s="16">
+        <v>5.3247231717396003E-2</v>
+      </c>
+      <c r="I5" s="16">
+        <v>4.8131507134494399E-2</v>
+      </c>
+      <c r="J5" s="22">
+        <v>3.07782721144347E-2</v>
+      </c>
+      <c r="K5" s="16">
+        <v>3.8775704713500503E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.42030612244897902</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.26989795918367299</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.70214285714285696</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.33754237288135502</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.27296610169491498</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0.77584745762711804</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0.465574712643678</v>
+      </c>
+      <c r="J6" s="22">
+        <v>0.30235632183908001</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.57316091954022896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.77799826094604196</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.62020439783213899</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1.5828214388510999</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.62251552075899197</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.44406453157364301</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1.7128279287707799</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0.90678588131344495</v>
+      </c>
+      <c r="J7" s="22">
+        <v>0.58275001748431798</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1.50771928421722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.442653061224489</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.30397959183673401</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.86918367346938696</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0.32313559322033802</v>
+      </c>
+      <c r="G8" s="22">
+        <v>0.31101694915254202</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.89593220338983004</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.39936781609195399</v>
+      </c>
+      <c r="J8" s="22">
+        <v>0.221954022988505</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.77224137931034398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="16">
+        <v>3.4571210016614298E-2</v>
+      </c>
+      <c r="D9" s="22">
+        <v>2.6167073600870599E-2</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.10117314187762599</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2.3734918246323799E-2</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1.7048962960689501E-2</v>
+      </c>
+      <c r="H9" s="16">
+        <v>9.5535675882812796E-2</v>
+      </c>
+      <c r="I9" s="16">
+        <v>3.1698973584203698E-2</v>
+      </c>
+      <c r="J9" s="22">
+        <v>2.1398556397482501E-2</v>
+      </c>
+      <c r="K9" s="16">
+        <v>8.7171942648499395E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.421122448979591</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.25040816326530602</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.73163265306122405</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0.234237288135593</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0.32618644067796598</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0.81449152542372805</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.269597701149425</v>
+      </c>
+      <c r="J10" s="22">
+        <v>0.22103448275862</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.64477011494252801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.13711927129367199</v>
+      </c>
+      <c r="D11" s="22">
+        <v>9.3415915168832395E-2</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.27602277931192498</v>
+      </c>
+      <c r="F11" s="22">
+        <v>7.1697541106708104E-2</v>
+      </c>
+      <c r="G11" s="16">
+        <v>8.83832328389757E-2</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0.26632559557493901</v>
+      </c>
+      <c r="I11" s="16">
+        <v>6.6735051407192603E-2</v>
+      </c>
+      <c r="J11" s="22">
+        <v>5.6989336459083398E-2</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.17943107792865501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0.145654580981328</v>
+      </c>
+      <c r="D12" s="22">
+        <v>6.0892314372557502E-2</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0.139381241858445</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0.102619004688063</v>
+      </c>
+      <c r="G12" s="22">
+        <v>6.4423007573025604E-2</v>
+      </c>
+      <c r="H12" s="16">
+        <v>9.2577533357374606E-2</v>
+      </c>
+      <c r="I12" s="16">
+        <v>6.2416238689166001E-2</v>
+      </c>
+      <c r="J12" s="22">
+        <v>4.39508437270726E-2</v>
+      </c>
+      <c r="K12" s="16">
+        <v>5.8095500122279202E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="16">
+        <v>5.3495188061392598E-2</v>
+      </c>
+      <c r="D13" s="22">
+        <v>3.5257503348294299E-2</v>
+      </c>
+      <c r="E13" s="16">
+        <v>5.1142718350508098E-2</v>
+      </c>
+      <c r="F13" s="16">
+        <v>4.3617524972792199E-2</v>
+      </c>
+      <c r="G13" s="22">
+        <v>2.8451457536020502E-2</v>
+      </c>
+      <c r="H13" s="16">
+        <v>4.25760552874902E-2</v>
+      </c>
+      <c r="I13" s="16">
+        <v>2.8953443445941099E-2</v>
+      </c>
+      <c r="J13" s="22">
+        <v>2.4955302053384299E-2</v>
+      </c>
+      <c r="K13" s="16">
+        <v>2.79823518034557E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="I2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C10:E10">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:E11">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:E12">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:E13">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:H10">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:H11">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:H12">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:H13">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:K10">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:K11">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:K12">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:K13">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:E4">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:E5">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:H4">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:H5">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:K4">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:K5">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:E6">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:E7">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:H6">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:H7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:K6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:K7">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:E8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:E9">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:H8">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:H9">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:K8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:K9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:H15"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,18 +2405,18 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="13">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13">
         <v>1</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13">
         <v>2</v>
       </c>
-      <c r="H1" s="11"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1086,7 +2450,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1112,7 +2476,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1136,7 +2500,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1162,7 +2526,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1186,7 +2550,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1212,7 +2576,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1236,7 +2600,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1262,7 +2626,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +2650,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1312,7 +2676,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
@@ -1336,7 +2700,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1801,7 +3165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -1818,21 +3182,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="13">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13">
         <v>1</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13">
         <v>2</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1875,7 +3239,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
@@ -1910,7 +3274,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -1943,7 +3307,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -1978,7 +3342,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2011,7 +3375,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
@@ -2046,7 +3410,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -2079,7 +3443,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
@@ -2114,7 +3478,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -2147,7 +3511,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -2182,7 +3546,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -2215,7 +3579,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -2248,7 +3612,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -2283,7 +3647,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -2316,7 +3680,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="13"/>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +3713,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
@@ -2384,7 +3748,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="13"/>
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -2417,7 +3781,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -2450,7 +3814,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
@@ -2485,7 +3849,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -2518,7 +3882,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Add figures for the load modelling
</commit_message>
<xml_diff>
--- a/metric_means_KMEANS_3clusters.xlsx
+++ b/metric_means_KMEANS_3clusters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20175334\Documents\PycharmProjects\monte_carlo_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E819435-7E3F-401D-80EC-FB44B3E7B2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CF4003-90BB-4382-B1DD-D49469ADA236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="25">
   <si>
     <t>cluster</t>
   </si>
@@ -96,13 +96,16 @@
   <si>
     <t>CSI</t>
   </si>
+  <si>
+    <t>Index</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -715,7 +718,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -724,6 +727,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,61 +805,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1154,440 +1166,482 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4342B8BF-6010-4EB9-B6B2-100D4AF52613}">
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.42578125" customWidth="1"/>
+    <col min="5" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.42578125" customWidth="1"/>
+    <col min="9" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1" customWidth="1"/>
+    <col min="13" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-    </row>
-    <row r="2" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="38" t="s">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-    </row>
-    <row r="3" spans="2:12" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+    </row>
+    <row r="3" spans="2:15" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="J3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="K3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="L3" s="29"/>
+      <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="N3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="O3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="29"/>
+      <c r="E4" s="25">
         <v>0.40693877551020402</v>
       </c>
-      <c r="E4" s="36">
+      <c r="F4" s="26">
         <v>0.28826530612244899</v>
       </c>
-      <c r="F4" s="35">
+      <c r="G4" s="25">
         <v>0.63551020408163195</v>
       </c>
-      <c r="G4" s="35">
+      <c r="H4" s="20"/>
+      <c r="I4" s="25">
         <v>0.50813559322033897</v>
       </c>
-      <c r="H4" s="36">
+      <c r="J4" s="26">
         <v>0.22906779661016899</v>
       </c>
-      <c r="I4" s="35">
+      <c r="K4" s="25">
         <v>0.69805084745762702</v>
       </c>
-      <c r="J4" s="35">
+      <c r="L4" s="20"/>
+      <c r="M4" s="25">
         <v>0.62040229885057396</v>
       </c>
-      <c r="K4" s="36">
+      <c r="N4" s="26">
         <v>0.42339080459770101</v>
       </c>
-      <c r="L4" s="35">
+      <c r="O4" s="25">
         <v>0.52126436781609198</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
-      <c r="C5" s="30" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
+      <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="29"/>
+      <c r="E5" s="27">
         <v>3.3478881648663E-2</v>
       </c>
-      <c r="E5" s="28">
+      <c r="F5" s="19">
         <v>2.1846556638083499E-2</v>
       </c>
-      <c r="F5" s="37">
+      <c r="G5" s="27">
         <v>5.43953492350637E-2</v>
       </c>
-      <c r="G5" s="37">
+      <c r="H5" s="20"/>
+      <c r="I5" s="27">
         <v>3.2396523384897298E-2</v>
       </c>
-      <c r="H5" s="28">
+      <c r="J5" s="19">
         <v>1.7171336125926601E-2</v>
       </c>
-      <c r="I5" s="37">
+      <c r="K5" s="27">
         <v>5.3247231717396003E-2</v>
       </c>
-      <c r="J5" s="37">
+      <c r="L5" s="20"/>
+      <c r="M5" s="27">
         <v>4.8131507134494399E-2</v>
       </c>
-      <c r="K5" s="28">
+      <c r="N5" s="19">
         <v>3.07782721144347E-2</v>
       </c>
-      <c r="L5" s="37">
+      <c r="O5" s="27">
         <v>3.8775704713500503E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="29"/>
+      <c r="E6" s="25">
         <v>0.42030612244897902</v>
       </c>
-      <c r="E6" s="36">
+      <c r="F6" s="26">
         <v>0.26989795918367299</v>
       </c>
-      <c r="F6" s="35">
+      <c r="G6" s="25">
         <v>0.70214285714285696</v>
       </c>
-      <c r="G6" s="35">
+      <c r="H6" s="20"/>
+      <c r="I6" s="25">
         <v>0.33754237288135502</v>
       </c>
-      <c r="H6" s="36">
+      <c r="J6" s="26">
         <v>0.27296610169491498</v>
       </c>
-      <c r="I6" s="35">
+      <c r="K6" s="25">
         <v>0.77584745762711804</v>
       </c>
-      <c r="J6" s="35">
+      <c r="L6" s="20"/>
+      <c r="M6" s="25">
         <v>0.465574712643678</v>
       </c>
-      <c r="K6" s="36">
+      <c r="N6" s="26">
         <v>0.30235632183908001</v>
       </c>
-      <c r="L6" s="35">
+      <c r="O6" s="25">
         <v>0.57316091954022896</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
-      <c r="C7" s="30" t="s">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
+      <c r="C7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="29"/>
+      <c r="E7" s="27">
         <v>0.77799826094604196</v>
       </c>
-      <c r="E7" s="28">
+      <c r="F7" s="19">
         <v>0.62020439783213899</v>
       </c>
-      <c r="F7" s="37">
+      <c r="G7" s="27">
         <v>1.5828214388510999</v>
       </c>
-      <c r="G7" s="37">
+      <c r="H7" s="20"/>
+      <c r="I7" s="27">
         <v>0.62251552075899197</v>
       </c>
-      <c r="H7" s="28">
+      <c r="J7" s="19">
         <v>0.44406453157364301</v>
       </c>
-      <c r="I7" s="37">
+      <c r="K7" s="27">
         <v>1.7128279287707799</v>
       </c>
-      <c r="J7" s="37">
+      <c r="L7" s="20"/>
+      <c r="M7" s="27">
         <v>0.90678588131344495</v>
       </c>
-      <c r="K7" s="28">
+      <c r="N7" s="19">
         <v>0.58275001748431798</v>
       </c>
-      <c r="L7" s="37">
+      <c r="O7" s="27">
         <v>1.50771928421722</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="29"/>
+      <c r="E8" s="15">
         <v>0.442653061224489</v>
       </c>
-      <c r="E8" s="24">
+      <c r="F8" s="16">
         <v>0.30397959183673401</v>
       </c>
-      <c r="F8" s="23">
+      <c r="G8" s="15">
         <v>0.86918367346938696</v>
       </c>
-      <c r="G8" s="23">
+      <c r="H8" s="20"/>
+      <c r="I8" s="15">
         <v>0.32313559322033802</v>
       </c>
-      <c r="H8" s="24">
+      <c r="J8" s="16">
         <v>0.31101694915254202</v>
       </c>
-      <c r="I8" s="23">
+      <c r="K8" s="15">
         <v>0.89593220338983004</v>
       </c>
-      <c r="J8" s="23">
+      <c r="L8" s="20"/>
+      <c r="M8" s="15">
         <v>0.39936781609195399</v>
       </c>
-      <c r="K8" s="24">
+      <c r="N8" s="16">
         <v>0.221954022988505</v>
       </c>
-      <c r="L8" s="23">
+      <c r="O8" s="15">
         <v>0.77224137931034398</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="19" t="s">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="36"/>
+      <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="29"/>
+      <c r="E9" s="15">
         <v>3.4571210016614298E-2</v>
       </c>
-      <c r="E9" s="24">
+      <c r="F9" s="16">
         <v>2.6167073600870599E-2</v>
       </c>
-      <c r="F9" s="23">
+      <c r="G9" s="15">
         <v>0.10117314187762599</v>
       </c>
-      <c r="G9" s="23">
+      <c r="H9" s="20"/>
+      <c r="I9" s="15">
         <v>2.3734918246323799E-2</v>
       </c>
-      <c r="H9" s="24">
+      <c r="J9" s="16">
         <v>1.7048962960689501E-2</v>
       </c>
-      <c r="I9" s="23">
+      <c r="K9" s="15">
         <v>9.5535675882812796E-2</v>
       </c>
-      <c r="J9" s="23">
+      <c r="L9" s="20"/>
+      <c r="M9" s="15">
         <v>3.1698973584203698E-2</v>
       </c>
-      <c r="K9" s="24">
+      <c r="N9" s="16">
         <v>2.1398556397482501E-2</v>
       </c>
-      <c r="L9" s="23">
+      <c r="O9" s="15">
         <v>8.7171942648499395E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="29"/>
+      <c r="E10" s="25">
         <v>0.421122448979591</v>
       </c>
-      <c r="E10" s="36">
+      <c r="F10" s="26">
         <v>0.25040816326530602</v>
       </c>
-      <c r="F10" s="35">
+      <c r="G10" s="25">
         <v>0.73163265306122405</v>
       </c>
-      <c r="G10" s="36">
+      <c r="H10" s="20"/>
+      <c r="I10" s="26">
         <v>0.234237288135593</v>
       </c>
-      <c r="H10" s="35">
+      <c r="J10" s="25">
         <v>0.32618644067796598</v>
       </c>
-      <c r="I10" s="35">
+      <c r="K10" s="25">
         <v>0.81449152542372805</v>
       </c>
-      <c r="J10" s="35">
+      <c r="L10" s="20"/>
+      <c r="M10" s="25">
         <v>0.269597701149425</v>
       </c>
-      <c r="K10" s="36">
+      <c r="N10" s="26">
         <v>0.22103448275862</v>
       </c>
-      <c r="L10" s="35">
+      <c r="O10" s="25">
         <v>0.64477011494252801</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
-      <c r="C11" s="30" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
+      <c r="C11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="29"/>
+      <c r="E11" s="27">
         <v>0.13711927129367199</v>
       </c>
-      <c r="E11" s="28">
+      <c r="F11" s="19">
         <v>9.3415915168832395E-2</v>
       </c>
-      <c r="F11" s="37">
+      <c r="G11" s="27">
         <v>0.27602277931192498</v>
       </c>
-      <c r="G11" s="28">
+      <c r="H11" s="20"/>
+      <c r="I11" s="19">
         <v>7.1697541106708104E-2</v>
       </c>
-      <c r="H11" s="37">
+      <c r="J11" s="27">
         <v>8.83832328389757E-2</v>
       </c>
-      <c r="I11" s="37">
+      <c r="K11" s="27">
         <v>0.26632559557493901</v>
       </c>
-      <c r="J11" s="37">
+      <c r="L11" s="20"/>
+      <c r="M11" s="27">
         <v>6.6735051407192603E-2</v>
       </c>
-      <c r="K11" s="28">
+      <c r="N11" s="19">
         <v>5.6989336459083398E-2</v>
       </c>
-      <c r="L11" s="37">
+      <c r="O11" s="27">
         <v>0.17943107792865501</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="29"/>
+      <c r="E12" s="20">
         <v>0.145654580981328</v>
       </c>
-      <c r="E12" s="27">
+      <c r="F12" s="18">
         <v>6.0892314372557502E-2</v>
       </c>
-      <c r="F12" s="29">
+      <c r="G12" s="20">
         <v>0.139381241858445</v>
       </c>
-      <c r="G12" s="29">
+      <c r="H12" s="20"/>
+      <c r="I12" s="20">
         <v>0.102619004688063</v>
       </c>
-      <c r="H12" s="27">
+      <c r="J12" s="18">
         <v>6.4423007573025604E-2</v>
       </c>
-      <c r="I12" s="29">
+      <c r="K12" s="20">
         <v>9.2577533357374606E-2</v>
       </c>
-      <c r="J12" s="29">
+      <c r="L12" s="20"/>
+      <c r="M12" s="20">
         <v>6.2416238689166001E-2</v>
       </c>
-      <c r="K12" s="27">
+      <c r="N12" s="18">
         <v>4.39508437270726E-2</v>
       </c>
-      <c r="L12" s="29">
+      <c r="O12" s="20">
         <v>5.8095500122279202E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
-      <c r="C13" s="42" t="s">
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="34"/>
+      <c r="C13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="30"/>
+      <c r="E13" s="23">
         <v>5.3495188061392598E-2</v>
       </c>
-      <c r="E13" s="34">
+      <c r="F13" s="24">
         <v>3.5257503348294299E-2</v>
       </c>
-      <c r="F13" s="33">
+      <c r="G13" s="23">
         <v>5.1142718350508098E-2</v>
       </c>
-      <c r="G13" s="33">
+      <c r="H13" s="23"/>
+      <c r="I13" s="23">
         <v>4.3617524972792199E-2</v>
       </c>
-      <c r="H13" s="34">
+      <c r="J13" s="24">
         <v>2.8451457536020502E-2</v>
       </c>
-      <c r="I13" s="33">
+      <c r="K13" s="23">
         <v>4.25760552874902E-2</v>
       </c>
-      <c r="J13" s="33">
+      <c r="L13" s="23"/>
+      <c r="M13" s="23">
         <v>2.8953443445941099E-2</v>
       </c>
-      <c r="K13" s="34">
+      <c r="N13" s="24">
         <v>2.4955302053384299E-2</v>
       </c>
-      <c r="L13" s="33">
+      <c r="O13" s="23">
         <v>2.79823518034557E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M2:O2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
@@ -1607,416 +1661,417 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="14" customWidth="1"/>
-    <col min="3" max="11" width="5.85546875" style="14" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="7" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="8" customWidth="1"/>
+    <col min="3" max="11" width="5.85546875" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="9">
         <v>0.40693877551020402</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="14">
         <v>0.28826530612244899</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="9">
         <v>0.63551020408163195</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="9">
         <v>0.50813559322033897</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="14">
         <v>0.22906779661016899</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="9">
         <v>0.69805084745762702</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="9">
         <v>0.62040229885057396</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="14">
         <v>0.42339080459770101</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="9">
         <v>0.52126436781609198</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="9">
         <v>3.3478881648663E-2</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="14">
         <v>2.1846556638083499E-2</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="9">
         <v>5.43953492350637E-2</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="9">
         <v>3.2396523384897298E-2</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="14">
         <v>1.7171336125926601E-2</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="9">
         <v>5.3247231717396003E-2</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="9">
         <v>4.8131507134494399E-2</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="14">
         <v>3.07782721144347E-2</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="9">
         <v>3.8775704713500503E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="9">
         <v>0.42030612244897902</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="14">
         <v>0.26989795918367299</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="9">
         <v>0.70214285714285696</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="9">
         <v>0.33754237288135502</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="14">
         <v>0.27296610169491498</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="9">
         <v>0.77584745762711804</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="9">
         <v>0.465574712643678</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="14">
         <v>0.30235632183908001</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="9">
         <v>0.57316091954022896</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="9">
         <v>0.77799826094604196</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="14">
         <v>0.62020439783213899</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="9">
         <v>1.5828214388510999</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="9">
         <v>0.62251552075899197</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="14">
         <v>0.44406453157364301</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="9">
         <v>1.7128279287707799</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="9">
         <v>0.90678588131344495</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="14">
         <v>0.58275001748431798</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="9">
         <v>1.50771928421722</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="9">
         <v>0.442653061224489</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="14">
         <v>0.30397959183673401</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="9">
         <v>0.86918367346938696</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="9">
         <v>0.32313559322033802</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="14">
         <v>0.31101694915254202</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="9">
         <v>0.89593220338983004</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="9">
         <v>0.39936781609195399</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="14">
         <v>0.221954022988505</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="9">
         <v>0.77224137931034398</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="9">
         <v>3.4571210016614298E-2</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="14">
         <v>2.6167073600870599E-2</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="9">
         <v>0.10117314187762599</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="9">
         <v>2.3734918246323799E-2</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="14">
         <v>1.7048962960689501E-2</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="9">
         <v>9.5535675882812796E-2</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="9">
         <v>3.1698973584203698E-2</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="14">
         <v>2.1398556397482501E-2</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="9">
         <v>8.7171942648499395E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="9">
         <v>0.421122448979591</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="14">
         <v>0.25040816326530602</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="9">
         <v>0.73163265306122405</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="14">
         <v>0.234237288135593</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="9">
         <v>0.32618644067796598</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="9">
         <v>0.81449152542372805</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="9">
         <v>0.269597701149425</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="14">
         <v>0.22103448275862</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="9">
         <v>0.64477011494252801</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="9">
         <v>0.13711927129367199</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="14">
         <v>9.3415915168832395E-2</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="9">
         <v>0.27602277931192498</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="14">
         <v>7.1697541106708104E-2</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="9">
         <v>8.83832328389757E-2</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="9">
         <v>0.26632559557493901</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="9">
         <v>6.6735051407192603E-2</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="14">
         <v>5.6989336459083398E-2</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="9">
         <v>0.17943107792865501</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="9">
         <v>0.145654580981328</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="14">
         <v>6.0892314372557502E-2</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="9">
         <v>0.139381241858445</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="9">
         <v>0.102619004688063</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="14">
         <v>6.4423007573025604E-2</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="9">
         <v>9.2577533357374606E-2</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="9">
         <v>6.2416238689166001E-2</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="14">
         <v>4.39508437270726E-2</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="9">
         <v>5.8095500122279202E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="37"/>
+      <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="9">
         <v>5.3495188061392598E-2</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="14">
         <v>3.5257503348294299E-2</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="9">
         <v>5.1142718350508098E-2</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="9">
         <v>4.3617524972792199E-2</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="14">
         <v>2.8451457536020502E-2</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="9">
         <v>4.25760552874902E-2</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="9">
         <v>2.8953443445941099E-2</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="14">
         <v>2.4955302053384299E-2</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="9">
         <v>2.79823518034557E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="I2:K2"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="C2:E2"/>
@@ -2024,7 +2079,6 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:E10">
     <cfRule type="colorScale" priority="60">
@@ -2405,18 +2459,18 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13">
+      <c r="C1" s="43">
         <v>0</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43">
         <v>1</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13">
+      <c r="F1" s="43"/>
+      <c r="G1" s="43">
         <v>2</v>
       </c>
-      <c r="H1" s="13"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2450,7 +2504,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="40" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2476,7 +2530,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2500,7 +2554,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2526,7 +2580,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -2550,7 +2604,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2576,7 +2630,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2600,7 +2654,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2626,7 +2680,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2650,7 +2704,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2676,7 +2730,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
@@ -2700,7 +2754,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -3182,21 +3236,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13">
+      <c r="C1" s="43">
         <v>0</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43">
         <v>1</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43">
         <v>2</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3239,7 +3293,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="43" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
@@ -3274,7 +3328,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="43"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -3307,7 +3361,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -3342,7 +3396,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="43"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -3375,7 +3429,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
@@ -3410,7 +3464,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="43"/>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -3443,7 +3497,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
@@ -3478,7 +3532,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="43"/>
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -3511,7 +3565,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="43" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -3546,7 +3600,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="43"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -3579,7 +3633,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="43"/>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -3612,7 +3666,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -3647,7 +3701,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="43"/>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -3680,7 +3734,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="43"/>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -3713,7 +3767,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
@@ -3748,7 +3802,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="43"/>
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -3781,7 +3835,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="43"/>
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -3814,7 +3868,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
@@ -3849,7 +3903,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="43"/>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -3882,7 +3936,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="43"/>
       <c r="B23" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Modified figure of clustering metrics and table
</commit_message>
<xml_diff>
--- a/metric_means_KMEANS_3clusters.xlsx
+++ b/metric_means_KMEANS_3clusters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20175334\Documents\PycharmProjects\monte_carlo_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CF4003-90BB-4382-B1DD-D49469ADA236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2604B3FE-B6EA-48DD-A865-B1824742B1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
@@ -718,7 +718,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -758,9 +758,6 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -804,12 +801,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1166,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4342B8BF-6010-4EB9-B6B2-100D4AF52613}">
-  <dimension ref="B1:O14"/>
+  <dimension ref="B1:L14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,18 +1168,15 @@
     <col min="1" max="1" width="0.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" customWidth="1"/>
-    <col min="5" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.42578125" customWidth="1"/>
-    <col min="9" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1" customWidth="1"/>
-    <col min="13" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1200,448 +1188,409 @@
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-    </row>
-    <row r="2" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="35" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="35" t="s">
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-    </row>
-    <row r="3" spans="2:15" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="2:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="25">
+      <c r="D4" s="25">
         <v>0.40693877551020402</v>
       </c>
-      <c r="F4" s="26">
+      <c r="E4" s="26">
         <v>0.28826530612244899</v>
       </c>
+      <c r="F4" s="25">
+        <v>0.63551020408163195</v>
+      </c>
       <c r="G4" s="25">
-        <v>0.63551020408163195</v>
-      </c>
-      <c r="H4" s="20"/>
+        <v>0.50813559322033897</v>
+      </c>
+      <c r="H4" s="26">
+        <v>0.22906779661016899</v>
+      </c>
       <c r="I4" s="25">
-        <v>0.50813559322033897</v>
-      </c>
-      <c r="J4" s="26">
-        <v>0.22906779661016899</v>
-      </c>
-      <c r="K4" s="25">
         <v>0.69805084745762702</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="25">
+      <c r="J4" s="25">
         <v>0.62040229885057396</v>
       </c>
-      <c r="N4" s="26">
+      <c r="K4" s="26">
         <v>0.42339080459770101</v>
       </c>
-      <c r="O4" s="25">
+      <c r="L4" s="25">
         <v>0.52126436781609198</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="32"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="31"/>
       <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="27">
+      <c r="D5" s="27">
         <v>3.3478881648663E-2</v>
       </c>
-      <c r="F5" s="19">
+      <c r="E5" s="19">
         <v>2.1846556638083499E-2</v>
       </c>
+      <c r="F5" s="27">
+        <v>5.43953492350637E-2</v>
+      </c>
       <c r="G5" s="27">
-        <v>5.43953492350637E-2</v>
-      </c>
-      <c r="H5" s="20"/>
+        <v>3.2396523384897298E-2</v>
+      </c>
+      <c r="H5" s="19">
+        <v>1.7171336125926601E-2</v>
+      </c>
       <c r="I5" s="27">
-        <v>3.2396523384897298E-2</v>
-      </c>
-      <c r="J5" s="19">
-        <v>1.7171336125926601E-2</v>
-      </c>
-      <c r="K5" s="27">
         <v>5.3247231717396003E-2</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="27">
+      <c r="J5" s="27">
         <v>4.8131507134494399E-2</v>
       </c>
-      <c r="N5" s="19">
+      <c r="K5" s="19">
         <v>3.07782721144347E-2</v>
       </c>
-      <c r="O5" s="27">
+      <c r="L5" s="27">
         <v>3.8775704713500503E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="25">
+      <c r="D6" s="25">
         <v>0.42030612244897902</v>
       </c>
-      <c r="F6" s="26">
+      <c r="E6" s="26">
         <v>0.26989795918367299</v>
       </c>
+      <c r="F6" s="25">
+        <v>0.70214285714285696</v>
+      </c>
       <c r="G6" s="25">
-        <v>0.70214285714285696</v>
-      </c>
-      <c r="H6" s="20"/>
+        <v>0.33754237288135502</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0.27296610169491498</v>
+      </c>
       <c r="I6" s="25">
-        <v>0.33754237288135502</v>
-      </c>
-      <c r="J6" s="26">
-        <v>0.27296610169491498</v>
-      </c>
-      <c r="K6" s="25">
         <v>0.77584745762711804</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="25">
+      <c r="J6" s="25">
         <v>0.465574712643678</v>
       </c>
-      <c r="N6" s="26">
+      <c r="K6" s="26">
         <v>0.30235632183908001</v>
       </c>
-      <c r="O6" s="25">
+      <c r="L6" s="25">
         <v>0.57316091954022896</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="31"/>
       <c r="C7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="27">
+      <c r="D7" s="27">
         <v>0.77799826094604196</v>
       </c>
-      <c r="F7" s="19">
+      <c r="E7" s="19">
         <v>0.62020439783213899</v>
       </c>
+      <c r="F7" s="27">
+        <v>1.5828214388510999</v>
+      </c>
       <c r="G7" s="27">
-        <v>1.5828214388510999</v>
-      </c>
-      <c r="H7" s="20"/>
+        <v>0.62251552075899197</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.44406453157364301</v>
+      </c>
       <c r="I7" s="27">
-        <v>0.62251552075899197</v>
-      </c>
-      <c r="J7" s="19">
-        <v>0.44406453157364301</v>
-      </c>
-      <c r="K7" s="27">
         <v>1.7128279287707799</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="27">
+      <c r="J7" s="27">
         <v>0.90678588131344495</v>
       </c>
-      <c r="N7" s="19">
+      <c r="K7" s="19">
         <v>0.58275001748431798</v>
       </c>
-      <c r="O7" s="27">
+      <c r="L7" s="27">
         <v>1.50771928421722</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="15">
+      <c r="D8" s="15">
         <v>0.442653061224489</v>
       </c>
-      <c r="F8" s="16">
+      <c r="E8" s="16">
         <v>0.30397959183673401</v>
       </c>
+      <c r="F8" s="15">
+        <v>0.86918367346938696</v>
+      </c>
       <c r="G8" s="15">
-        <v>0.86918367346938696</v>
-      </c>
-      <c r="H8" s="20"/>
+        <v>0.32313559322033802</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.31101694915254202</v>
+      </c>
       <c r="I8" s="15">
-        <v>0.32313559322033802</v>
-      </c>
-      <c r="J8" s="16">
-        <v>0.31101694915254202</v>
-      </c>
-      <c r="K8" s="15">
         <v>0.89593220338983004</v>
       </c>
-      <c r="L8" s="20"/>
-      <c r="M8" s="15">
+      <c r="J8" s="15">
         <v>0.39936781609195399</v>
       </c>
-      <c r="N8" s="16">
+      <c r="K8" s="16">
         <v>0.221954022988505</v>
       </c>
-      <c r="O8" s="15">
+      <c r="L8" s="15">
         <v>0.77224137931034398</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
       <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="15">
+      <c r="D9" s="15">
         <v>3.4571210016614298E-2</v>
       </c>
-      <c r="F9" s="16">
+      <c r="E9" s="16">
         <v>2.6167073600870599E-2</v>
       </c>
+      <c r="F9" s="15">
+        <v>0.10117314187762599</v>
+      </c>
       <c r="G9" s="15">
-        <v>0.10117314187762599</v>
-      </c>
-      <c r="H9" s="20"/>
+        <v>2.3734918246323799E-2</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1.7048962960689501E-2</v>
+      </c>
       <c r="I9" s="15">
-        <v>2.3734918246323799E-2</v>
-      </c>
-      <c r="J9" s="16">
-        <v>1.7048962960689501E-2</v>
-      </c>
-      <c r="K9" s="15">
         <v>9.5535675882812796E-2</v>
       </c>
-      <c r="L9" s="20"/>
-      <c r="M9" s="15">
+      <c r="J9" s="15">
         <v>3.1698973584203698E-2</v>
       </c>
-      <c r="N9" s="16">
+      <c r="K9" s="16">
         <v>2.1398556397482501E-2</v>
       </c>
-      <c r="O9" s="15">
+      <c r="L9" s="15">
         <v>8.7171942648499395E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="25">
+      <c r="D10" s="25">
         <v>0.421122448979591</v>
       </c>
-      <c r="F10" s="26">
+      <c r="E10" s="26">
         <v>0.25040816326530602</v>
       </c>
-      <c r="G10" s="25">
+      <c r="F10" s="25">
         <v>0.73163265306122405</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="26">
+      <c r="G10" s="26">
         <v>0.234237288135593</v>
       </c>
+      <c r="H10" s="25">
+        <v>0.32618644067796598</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.81449152542372805</v>
+      </c>
       <c r="J10" s="25">
-        <v>0.32618644067796598</v>
-      </c>
-      <c r="K10" s="25">
-        <v>0.81449152542372805</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="25">
         <v>0.269597701149425</v>
       </c>
-      <c r="N10" s="26">
+      <c r="K10" s="26">
         <v>0.22103448275862</v>
       </c>
-      <c r="O10" s="25">
+      <c r="L10" s="25">
         <v>0.64477011494252801</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
       <c r="C11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="27">
+      <c r="D11" s="27">
         <v>0.13711927129367199</v>
       </c>
-      <c r="F11" s="19">
+      <c r="E11" s="19">
         <v>9.3415915168832395E-2</v>
       </c>
-      <c r="G11" s="27">
+      <c r="F11" s="27">
         <v>0.27602277931192498</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="19">
+      <c r="G11" s="19">
         <v>7.1697541106708104E-2</v>
       </c>
+      <c r="H11" s="27">
+        <v>8.83832328389757E-2</v>
+      </c>
+      <c r="I11" s="27">
+        <v>0.26632559557493901</v>
+      </c>
       <c r="J11" s="27">
-        <v>8.83832328389757E-2</v>
-      </c>
-      <c r="K11" s="27">
-        <v>0.26632559557493901</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="27">
         <v>6.6735051407192603E-2</v>
       </c>
-      <c r="N11" s="19">
+      <c r="K11" s="19">
         <v>5.6989336459083398E-2</v>
       </c>
-      <c r="O11" s="27">
+      <c r="L11" s="27">
         <v>0.17943107792865501</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="s">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="20">
+      <c r="D12" s="20">
         <v>0.145654580981328</v>
       </c>
-      <c r="F12" s="18">
+      <c r="E12" s="18">
         <v>6.0892314372557502E-2</v>
       </c>
+      <c r="F12" s="20">
+        <v>0.139381241858445</v>
+      </c>
       <c r="G12" s="20">
-        <v>0.139381241858445</v>
-      </c>
-      <c r="H12" s="20"/>
+        <v>0.102619004688063</v>
+      </c>
+      <c r="H12" s="18">
+        <v>6.4423007573025604E-2</v>
+      </c>
       <c r="I12" s="20">
-        <v>0.102619004688063</v>
-      </c>
-      <c r="J12" s="18">
-        <v>6.4423007573025604E-2</v>
-      </c>
-      <c r="K12" s="20">
         <v>9.2577533357374606E-2</v>
       </c>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20">
+      <c r="J12" s="20">
         <v>6.2416238689166001E-2</v>
       </c>
-      <c r="N12" s="18">
+      <c r="K12" s="18">
         <v>4.39508437270726E-2</v>
       </c>
-      <c r="O12" s="20">
+      <c r="L12" s="20">
         <v>5.8095500122279202E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="34"/>
-      <c r="C13" s="30" t="s">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="33"/>
+      <c r="C13" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="23">
+      <c r="D13" s="23">
         <v>5.3495188061392598E-2</v>
       </c>
-      <c r="F13" s="24">
+      <c r="E13" s="24">
         <v>3.5257503348294299E-2</v>
       </c>
+      <c r="F13" s="23">
+        <v>5.1142718350508098E-2</v>
+      </c>
       <c r="G13" s="23">
-        <v>5.1142718350508098E-2</v>
-      </c>
-      <c r="H13" s="23"/>
+        <v>4.3617524972792199E-2</v>
+      </c>
+      <c r="H13" s="24">
+        <v>2.8451457536020502E-2</v>
+      </c>
       <c r="I13" s="23">
-        <v>4.3617524972792199E-2</v>
-      </c>
-      <c r="J13" s="24">
-        <v>2.8451457536020502E-2</v>
-      </c>
-      <c r="K13" s="23">
         <v>4.25760552874902E-2</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23">
+      <c r="J13" s="23">
         <v>2.8953443445941099E-2</v>
       </c>
-      <c r="N13" s="24">
+      <c r="K13" s="24">
         <v>2.4955302053384299E-2</v>
       </c>
-      <c r="O13" s="23">
+      <c r="L13" s="23">
         <v>2.79823518034557E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
@@ -1678,21 +1627,21 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -1730,7 +1679,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1765,7 +1714,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -1798,7 +1747,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1833,7 +1782,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -1866,7 +1815,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1901,7 +1850,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
@@ -1934,7 +1883,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1969,7 +1918,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
@@ -2002,7 +1951,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -2037,7 +1986,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
@@ -2459,18 +2408,18 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43">
+      <c r="C1" s="42">
         <v>0</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42">
         <v>1</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42">
         <v>2</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2504,7 +2453,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2530,7 +2479,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2554,7 +2503,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2580,7 +2529,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -2604,7 +2553,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2630,7 +2579,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2654,7 +2603,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2680,7 +2629,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2704,7 +2653,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2730,7 +2679,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
@@ -2754,7 +2703,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -3236,21 +3185,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43">
+      <c r="C1" s="42">
         <v>0</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42">
         <v>1</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43">
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42">
         <v>2</v>
       </c>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3293,7 +3242,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
@@ -3328,7 +3277,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
+      <c r="A5" s="42"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -3361,7 +3310,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -3396,7 +3345,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="42"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -3429,7 +3378,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
@@ -3464,7 +3413,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="42"/>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -3497,7 +3446,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
@@ -3532,7 +3481,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="42"/>
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -3565,7 +3514,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -3600,7 +3549,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="42"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -3633,7 +3582,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="42"/>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -3666,7 +3615,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -3701,7 +3650,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
+      <c r="A16" s="42"/>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -3734,7 +3683,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="42"/>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -3767,7 +3716,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
@@ -3802,7 +3751,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="42"/>
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -3835,7 +3784,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
+      <c r="A20" s="42"/>
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -3868,7 +3817,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
@@ -3903,7 +3852,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
+      <c r="A22" s="42"/>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -3936,7 +3885,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+      <c r="A23" s="42"/>
       <c r="B23" t="s">
         <v>11</v>
       </c>

</xml_diff>